<commit_message>
Rename data organization files and add some for emoreact
</commit_message>
<xml_diff>
--- a/datasets/EmoReact_V_1.0/usable_info.xlsx
+++ b/datasets/EmoReact_V_1.0/usable_info.xlsx
@@ -1,24 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michen\OneDrive - University of North Carolina at Chapel Hill\Desktop\multilingual_speech_valence_classification\datasets\EmoReact_V_1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC84D368-8436-4804-9131-403D34E9BEF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CB9D6F-D5D4-4A3A-94D4-FAAC53F95547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{8EAFB4F7-9D7F-478B-B4F8-E57320AF50D7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{8EAFB4F7-9D7F-478B-B4F8-E57320AF50D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$D$1103</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="66" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -10091,7 +10094,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5DC1BF8E-F051-4BBC-B5E6-BE17039912BE}" name="PivotTable26" cacheId="66" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5DC1BF8E-F051-4BBC-B5E6-BE17039912BE}" name="PivotTable26" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField dataField="1" showAll="0"/>
@@ -10440,7 +10443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED29463-AADD-401A-BD57-AA00FB8F5CB1}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -10504,7 +10507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB98C27-F24D-40BA-8C32-93A1E747C5E0}">
   <dimension ref="A1:D1103"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -27056,6 +27059,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D1103" xr:uid="{3CB98C27-F24D-40BA-8C32-93A1E747C5E0}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>